<commit_message>
link may be empty
</commit_message>
<xml_diff>
--- a/avito_78404_tst.xlsx
+++ b/avito_78404_tst.xlsx
@@ -110,7 +110,7 @@
     <t>2020-03-22 06:11:00</t>
   </si>
   <si>
-    <t>https://19.img.avito.st/1280x960/8342933419.jpg, https://51.img.avito.st/1280x960/8318818051.jpg, https://38.img.avito.st/1280x960/8318818038.jpg, https://54.img.avito.st/1280x960/8318818054.jpg</t>
+    <t>https://19.img.avito.st/1280x960/8342933419.jpg, , https://51.img.avito.st/1280x960/8318818051.jpg, https://38.img.avito.st/1280x960/8318818038.jpg, https://54.img.avito.st/1280x960/8318818054.jpg</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>